<commit_message>
Mobile Field added, try to run parallel
</commit_message>
<xml_diff>
--- a/Verifies.xlsx
+++ b/Verifies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FullName" sheetId="3" r:id="rId1"/>
@@ -12,14 +12,15 @@
     <sheet name="Password" sheetId="11" r:id="rId3"/>
     <sheet name="ConfirmPassword" sheetId="12" r:id="rId4"/>
     <sheet name="Email" sheetId="13" r:id="rId5"/>
-    <sheet name="Mobile" sheetId="14" r:id="rId6"/>
+    <sheet name="EmailSuccess" sheetId="15" r:id="rId6"/>
+    <sheet name="Mobile" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="121">
   <si>
     <t>Empty</t>
   </si>
@@ -87,24 +88,6 @@
     <t>Тестер</t>
   </si>
   <si>
-    <t>Splendor</t>
-  </si>
-  <si>
-    <t>Nymgo</t>
-  </si>
-  <si>
-    <t>Ahwar</t>
-  </si>
-  <si>
-    <t>Callback</t>
-  </si>
-  <si>
-    <t>Free</t>
-  </si>
-  <si>
-    <t>Voip</t>
-  </si>
-  <si>
     <t>Reserved</t>
   </si>
   <si>
@@ -175,6 +158,231 @@
   </si>
   <si>
     <t>InvalidDomain</t>
+  </si>
+  <si>
+    <t>0123456789@test.com</t>
+  </si>
+  <si>
+    <t>e^mail@test.com</t>
+  </si>
+  <si>
+    <t>e!mail@test.com</t>
+  </si>
+  <si>
+    <t>e#mail@test.com</t>
+  </si>
+  <si>
+    <t>e$mail@test.com</t>
+  </si>
+  <si>
+    <t>e%mail@test.com</t>
+  </si>
+  <si>
+    <t>e&amp;mail@test.com</t>
+  </si>
+  <si>
+    <t>e*mail@test.com</t>
+  </si>
+  <si>
+    <t>e(mail@test.com</t>
+  </si>
+  <si>
+    <t>e)mail@test.com</t>
+  </si>
+  <si>
+    <t>e+mail@test.com</t>
+  </si>
+  <si>
+    <t>e=mail@test.com</t>
+  </si>
+  <si>
+    <t>e;mail@test.com</t>
+  </si>
+  <si>
+    <t>e:mail@test.com</t>
+  </si>
+  <si>
+    <t>e&lt;mail@test.com</t>
+  </si>
+  <si>
+    <t>e&gt;mail@test.com</t>
+  </si>
+  <si>
+    <t>e,mail@test.com</t>
+  </si>
+  <si>
+    <t>e/mail@test.com</t>
+  </si>
+  <si>
+    <t>e\mail@test.com</t>
+  </si>
+  <si>
+    <t>e[mail@test.com</t>
+  </si>
+  <si>
+    <t>e]mail@test.com</t>
+  </si>
+  <si>
+    <t>e{mail@test.com</t>
+  </si>
+  <si>
+    <t>e}mail@test.com</t>
+  </si>
+  <si>
+    <t>TESTEMAIL@TEST.COM</t>
+  </si>
+  <si>
+    <t>testemail@test.com</t>
+  </si>
+  <si>
+    <t>e.mail@test.com</t>
+  </si>
+  <si>
+    <t>e_mail@test.com</t>
+  </si>
+  <si>
+    <t>e-mail@test.com</t>
+  </si>
+  <si>
+    <t>.email@test.com</t>
+  </si>
+  <si>
+    <t>email@test.com.</t>
+  </si>
+  <si>
+    <t>e..mail@test.com</t>
+  </si>
+  <si>
+    <t>test@test.test</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>SplendorEmail@test.com</t>
+  </si>
+  <si>
+    <t>NymgoEmail@test.com</t>
+  </si>
+  <si>
+    <t>AhwarEmail@test.com</t>
+  </si>
+  <si>
+    <t>CallbackEmail@test.com</t>
+  </si>
+  <si>
+    <t>FreeEmail@test.com</t>
+  </si>
+  <si>
+    <t>VoipEmail@test.com</t>
+  </si>
+  <si>
+    <t>e mail@test.com</t>
+  </si>
+  <si>
+    <t>SplendorName</t>
+  </si>
+  <si>
+    <t>NymgoName</t>
+  </si>
+  <si>
+    <t>AhwarName</t>
+  </si>
+  <si>
+    <t>CallbackName</t>
+  </si>
+  <si>
+    <t>FreeName</t>
+  </si>
+  <si>
+    <t>VoipName</t>
+  </si>
+  <si>
+    <t>InvalidPattern</t>
+  </si>
+  <si>
+    <t>111111111111111111111</t>
+  </si>
+  <si>
+    <t>a1111111</t>
+  </si>
+  <si>
+    <t>!1111111</t>
+  </si>
+  <si>
+    <t>@111111</t>
+  </si>
+  <si>
+    <t>#1111111</t>
+  </si>
+  <si>
+    <t>$1111111</t>
+  </si>
+  <si>
+    <t>%1111111</t>
+  </si>
+  <si>
+    <t>^1111111</t>
+  </si>
+  <si>
+    <t>&amp;1111111</t>
+  </si>
+  <si>
+    <t>*1111111</t>
+  </si>
+  <si>
+    <t>(1111111</t>
+  </si>
+  <si>
+    <t>)1111111</t>
+  </si>
+  <si>
+    <t>{1111111</t>
+  </si>
+  <si>
+    <t>}1111111</t>
+  </si>
+  <si>
+    <t>[1111111</t>
+  </si>
+  <si>
+    <t>]1111111</t>
+  </si>
+  <si>
+    <t>:1111111</t>
+  </si>
+  <si>
+    <t>;1111111</t>
+  </si>
+  <si>
+    <t>"1111111</t>
+  </si>
+  <si>
+    <t>\1111111</t>
+  </si>
+  <si>
+    <t>/1111111</t>
+  </si>
+  <si>
+    <t>&lt;1111111</t>
+  </si>
+  <si>
+    <t>&gt;1111111</t>
+  </si>
+  <si>
+    <t>1'111111</t>
+  </si>
+  <si>
+    <t>.1111111</t>
+  </si>
+  <si>
+    <t>-1111111</t>
+  </si>
+  <si>
+    <t>=1111111</t>
+  </si>
+  <si>
+    <t>_1111111</t>
   </si>
 </sst>
 </file>
@@ -210,9 +418,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,7 +792,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,58 +881,58 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -753,18 +963,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -772,7 +982,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,23 +990,23 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -826,26 +1036,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -855,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,104 +1085,274 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -982,10 +1362,77 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,107 +1449,238 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>92</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1111111</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>92</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>92</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>92</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>92</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>92</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>92</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>